<commit_message>
Update all data and inventory files
</commit_message>
<xml_diff>
--- a/data/inventories/sonde_sensor_df_describe_stats.xlsx
+++ b/data/inventories/sonde_sensor_df_describe_stats.xlsx
@@ -535,64 +535,64 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1217328</v>
+        <v>1233387</v>
       </c>
       <c r="C2" t="n">
-        <v>1217328</v>
+        <v>1233387</v>
       </c>
       <c r="D2" t="n">
-        <v>1217328</v>
+        <v>1233387</v>
       </c>
       <c r="E2" t="n">
-        <v>1217328</v>
+        <v>1233387</v>
       </c>
       <c r="F2" t="n">
-        <v>864529</v>
+        <v>880588</v>
       </c>
       <c r="G2" t="n">
-        <v>864529</v>
+        <v>880588</v>
       </c>
       <c r="H2" t="n">
-        <v>1161728</v>
+        <v>1177787</v>
       </c>
       <c r="I2" t="n">
-        <v>1161728</v>
+        <v>1177787</v>
       </c>
       <c r="J2" t="n">
-        <v>1164806</v>
+        <v>1180865</v>
       </c>
       <c r="K2" t="n">
-        <v>1164811</v>
+        <v>1180870</v>
       </c>
       <c r="L2" t="n">
-        <v>1164811</v>
+        <v>1180870</v>
       </c>
       <c r="M2" t="n">
-        <v>1164811</v>
+        <v>1180870</v>
       </c>
       <c r="N2" t="n">
-        <v>1164811</v>
+        <v>1180870</v>
       </c>
       <c r="O2" t="n">
-        <v>774046</v>
+        <v>790105</v>
       </c>
       <c r="P2" t="n">
-        <v>1170784</v>
+        <v>1186843</v>
       </c>
       <c r="Q2" t="n">
-        <v>1170784</v>
+        <v>1186843</v>
       </c>
       <c r="R2" t="n">
-        <v>1147037</v>
+        <v>1163096</v>
       </c>
       <c r="S2" t="n">
-        <v>1147037</v>
+        <v>1163096</v>
       </c>
       <c r="T2" t="n">
-        <v>1156380</v>
+        <v>1172439</v>
       </c>
       <c r="U2" t="n">
-        <v>721133</v>
+        <v>737192</v>
       </c>
       <c r="V2" t="n">
         <v>0</v>
@@ -607,22 +607,22 @@
         <v>13693</v>
       </c>
       <c r="Z2" t="n">
-        <v>67996</v>
+        <v>84055</v>
       </c>
       <c r="AA2" t="n">
-        <v>67996</v>
+        <v>84055</v>
       </c>
       <c r="AB2" t="n">
-        <v>83442</v>
+        <v>99501</v>
       </c>
       <c r="AC2" t="n">
-        <v>83442</v>
+        <v>99501</v>
       </c>
       <c r="AD2" t="n">
-        <v>67395</v>
+        <v>83454</v>
       </c>
       <c r="AE2" t="n">
-        <v>67395</v>
+        <v>83454</v>
       </c>
       <c r="AF2" t="n">
         <v>16047</v>
@@ -641,61 +641,61 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>0.006519196141056478</v>
+        <v>0.006434314614958647</v>
       </c>
       <c r="D3" t="n">
-        <v>5.191051220377744</v>
+        <v>5.187337226677433</v>
       </c>
       <c r="E3" t="n">
-        <v>0.5059345550254328</v>
+        <v>0.4999808656974656</v>
       </c>
       <c r="F3" t="n">
-        <v>76.61499024324226</v>
+        <v>76.45911413737184</v>
       </c>
       <c r="G3" t="n">
-        <v>5.805951090131157</v>
+        <v>5.793132168505588</v>
       </c>
       <c r="H3" t="n">
-        <v>1.506969281966176</v>
+        <v>1.527495930928089</v>
       </c>
       <c r="I3" t="n">
-        <v>41.36747650052336</v>
+        <v>41.4027450464303</v>
       </c>
       <c r="J3" t="n">
-        <v>29.92055434724752</v>
+        <v>29.9279669699754</v>
       </c>
       <c r="K3" t="n">
-        <v>49.22736933287892</v>
+        <v>49.05968802662446</v>
       </c>
       <c r="L3" t="n">
-        <v>45.0713283957655</v>
+        <v>44.91276338631688</v>
       </c>
       <c r="M3" t="n">
-        <v>0.01785252714818113</v>
+        <v>0.01776111680371252</v>
       </c>
       <c r="N3" t="n">
-        <v>44.54025477094567</v>
+        <v>44.38360276745112</v>
       </c>
       <c r="O3" t="n">
-        <v>31.19249631158872</v>
+        <v>30.99938362622689</v>
       </c>
       <c r="P3" t="n">
-        <v>6.869126217987262</v>
+        <v>6.872355265186717</v>
       </c>
       <c r="Q3" t="n">
-        <v>-9.095541705387161</v>
+        <v>-11.22799637357258</v>
       </c>
       <c r="R3" t="n">
-        <v>119.0747600992819</v>
+        <v>120.8834456485105</v>
       </c>
       <c r="S3" t="n">
-        <v>119.5902196703332</v>
+        <v>121.3917882100876</v>
       </c>
       <c r="T3" t="n">
-        <v>0.2208395968453277</v>
+        <v>0.2172730913932409</v>
       </c>
       <c r="U3" t="n">
-        <v>0.2475339126069671</v>
+        <v>0.2415331880975377</v>
       </c>
       <c r="V3" t="inlineStr"/>
       <c r="W3" t="n">
@@ -708,22 +708,22 @@
         <v>6.304643248375082</v>
       </c>
       <c r="Z3" t="n">
-        <v>54.58688672863109</v>
+        <v>51.11499518172625</v>
       </c>
       <c r="AA3" t="n">
         <v>0</v>
       </c>
       <c r="AB3" t="n">
-        <v>0.1825006591404808</v>
+        <v>0.1856417523441976</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.7300475779583423</v>
+        <v>0.7426145465874715</v>
       </c>
       <c r="AD3" t="n">
-        <v>-1.318506417390014</v>
+        <v>-1.308756560500395</v>
       </c>
       <c r="AE3" t="n">
-        <v>-1.318506417390014</v>
+        <v>-1.308756560500395</v>
       </c>
       <c r="AF3" t="n">
         <v>0.4289269022247149</v>
@@ -742,61 +742,61 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1613514983888754</v>
+        <v>0.1602993415109999</v>
       </c>
       <c r="D4" t="n">
-        <v>0.4645016073256546</v>
+        <v>0.4663718094485888</v>
       </c>
       <c r="E4" t="n">
-        <v>2.342708699218051</v>
+        <v>2.329541842772553</v>
       </c>
       <c r="F4" t="n">
-        <v>18.98058483879196</v>
+        <v>18.85408367187142</v>
       </c>
       <c r="G4" t="n">
-        <v>1.387962448044137</v>
+        <v>1.379365628991676</v>
       </c>
       <c r="H4" t="n">
-        <v>9.680887160383808</v>
+        <v>9.617589749684138</v>
       </c>
       <c r="I4" t="n">
-        <v>297.4499382788194</v>
+        <v>295.4156733617752</v>
       </c>
       <c r="J4" t="n">
-        <v>1.138188239209565</v>
+        <v>1.133147246058553</v>
       </c>
       <c r="K4" t="n">
-        <v>16.71224787911366</v>
+        <v>16.67047149207881</v>
       </c>
       <c r="L4" t="n">
-        <v>39.89380754351548</v>
+        <v>39.64843055222235</v>
       </c>
       <c r="M4" t="n">
-        <v>0.08382833817492147</v>
+        <v>0.08326084214932858</v>
       </c>
       <c r="N4" t="n">
-        <v>15.11131712127997</v>
+        <v>15.07719484408269</v>
       </c>
       <c r="O4" t="n">
-        <v>12.03633085345778</v>
+        <v>11.99670803555847</v>
       </c>
       <c r="P4" t="n">
-        <v>0.460617619939844</v>
+        <v>0.4593285532382717</v>
       </c>
       <c r="Q4" t="n">
-        <v>34.67947260319649</v>
+        <v>38.99206074345924</v>
       </c>
       <c r="R4" t="n">
-        <v>139.5183607119968</v>
+        <v>139.4460658705729</v>
       </c>
       <c r="S4" t="n">
-        <v>442.7141726523176</v>
+        <v>439.9277863798377</v>
       </c>
       <c r="T4" t="n">
-        <v>2.040354734126164</v>
+        <v>2.026561153747536</v>
       </c>
       <c r="U4" t="n">
-        <v>1.815519305056277</v>
+        <v>1.796087800601487</v>
       </c>
       <c r="V4" t="inlineStr"/>
       <c r="W4" t="n">
@@ -809,22 +809,22 @@
         <v>0.6375375308886371</v>
       </c>
       <c r="Z4" t="n">
-        <v>53.62711608907982</v>
+        <v>49.24392449555241</v>
       </c>
       <c r="AA4" t="n">
         <v>0</v>
       </c>
       <c r="AB4" t="n">
-        <v>0.2422132969558564</v>
+        <v>0.224440663687808</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.968771491228</v>
+        <v>0.897674536300694</v>
       </c>
       <c r="AD4" t="n">
-        <v>0.6166646683351502</v>
+        <v>0.5557555302600938</v>
       </c>
       <c r="AE4" t="n">
-        <v>0.6166646683351502</v>
+        <v>0.5557555302600938</v>
       </c>
       <c r="AF4" t="n">
         <v>0.1582026843063019</v>
@@ -953,31 +953,31 @@
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>59.3</v>
+        <v>59.6</v>
       </c>
       <c r="G6" t="n">
-        <v>4.56</v>
+        <v>4.58</v>
       </c>
       <c r="H6" t="n">
-        <v>-2</v>
+        <v>-1.88</v>
       </c>
       <c r="I6" t="n">
-        <v>29.87</v>
+        <v>30.34</v>
       </c>
       <c r="J6" t="n">
-        <v>29.169</v>
+        <v>29.181</v>
       </c>
       <c r="K6" t="n">
-        <v>46.4</v>
+        <v>45</v>
       </c>
       <c r="L6" t="n">
-        <v>43</v>
+        <v>41.5</v>
       </c>
       <c r="M6" t="n">
         <v>0.02</v>
       </c>
       <c r="N6" t="n">
-        <v>42.4</v>
+        <v>41</v>
       </c>
       <c r="O6" t="n">
         <v>20</v>
@@ -986,19 +986,19 @@
         <v>6.66</v>
       </c>
       <c r="Q6" t="n">
-        <v>-17.6</v>
+        <v>-17.7</v>
       </c>
       <c r="R6" t="n">
-        <v>33.1</v>
+        <v>33.5</v>
       </c>
       <c r="S6" t="n">
-        <v>33.1</v>
+        <v>33.5</v>
       </c>
       <c r="T6" t="n">
-        <v>-0.013</v>
+        <v>-0.014</v>
       </c>
       <c r="U6" t="n">
-        <v>-0.007</v>
+        <v>-0.008999999999999999</v>
       </c>
       <c r="V6" t="inlineStr"/>
       <c r="W6" t="n">
@@ -1011,22 +1011,22 @@
         <v>5.78</v>
       </c>
       <c r="Z6" t="n">
-        <v>28.33</v>
+        <v>27.85</v>
       </c>
       <c r="AA6" t="n">
         <v>0</v>
       </c>
       <c r="AB6" t="n">
-        <v>0.04</v>
+        <v>0.06</v>
       </c>
       <c r="AC6" t="n">
-        <v>0.16</v>
+        <v>0.24</v>
       </c>
       <c r="AD6" t="n">
-        <v>-1.81</v>
+        <v>-1.32</v>
       </c>
       <c r="AE6" t="n">
-        <v>-1.81</v>
+        <v>-1.32</v>
       </c>
       <c r="AF6" t="n">
         <v>0.32</v>
@@ -1054,25 +1054,25 @@
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>85.40000000000001</v>
+        <v>84.90000000000001</v>
       </c>
       <c r="G7" t="n">
-        <v>6.45</v>
+        <v>6.42</v>
       </c>
       <c r="H7" t="n">
-        <v>2.45</v>
+        <v>2.49</v>
       </c>
       <c r="I7" t="n">
-        <v>42.06</v>
+        <v>42.2</v>
       </c>
       <c r="J7" t="n">
-        <v>30.201</v>
+        <v>30.205</v>
       </c>
       <c r="K7" t="n">
-        <v>55.8</v>
+        <v>55.7</v>
       </c>
       <c r="L7" t="n">
-        <v>51.4</v>
+        <v>51.2</v>
       </c>
       <c r="M7" t="n">
         <v>0.02</v>
@@ -1084,22 +1084,22 @@
         <v>38</v>
       </c>
       <c r="P7" t="n">
-        <v>6.93</v>
+        <v>6.94</v>
       </c>
       <c r="Q7" t="n">
-        <v>-13.9</v>
+        <v>-14.1</v>
       </c>
       <c r="R7" t="n">
-        <v>49.4</v>
+        <v>50.1</v>
       </c>
       <c r="S7" t="n">
-        <v>49.4</v>
+        <v>50.1</v>
       </c>
       <c r="T7" t="n">
-        <v>0.013</v>
+        <v>0.012</v>
       </c>
       <c r="U7" t="n">
-        <v>0.021</v>
+        <v>0.02</v>
       </c>
       <c r="V7" t="inlineStr"/>
       <c r="W7" t="n">
@@ -1112,22 +1112,22 @@
         <v>6.26</v>
       </c>
       <c r="Z7" t="n">
-        <v>44.555</v>
+        <v>39.58</v>
       </c>
       <c r="AA7" t="n">
         <v>0</v>
       </c>
       <c r="AB7" t="n">
-        <v>0.12</v>
+        <v>0.14</v>
       </c>
       <c r="AC7" t="n">
-        <v>0.49</v>
+        <v>0.54</v>
       </c>
       <c r="AD7" t="n">
-        <v>-1.22</v>
+        <v>-1.24</v>
       </c>
       <c r="AE7" t="n">
-        <v>-1.22</v>
+        <v>-1.24</v>
       </c>
       <c r="AF7" t="n">
         <v>0.4</v>
@@ -1155,19 +1155,19 @@
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>91.09999999999999</v>
+        <v>91</v>
       </c>
       <c r="G8" t="n">
-        <v>6.84</v>
+        <v>6.83</v>
       </c>
       <c r="H8" t="n">
-        <v>5.4</v>
+        <v>5.28</v>
       </c>
       <c r="I8" t="n">
-        <v>49.7</v>
+        <v>49.41</v>
       </c>
       <c r="J8" t="n">
-        <v>30.499</v>
+        <v>30.501</v>
       </c>
       <c r="K8" t="n">
         <v>61</v>
@@ -1188,19 +1188,19 @@
         <v>7</v>
       </c>
       <c r="Q8" t="n">
-        <v>11.8</v>
+        <v>11.7</v>
       </c>
       <c r="R8" t="n">
-        <v>231.7</v>
+        <v>235.2</v>
       </c>
       <c r="S8" t="n">
-        <v>231.7</v>
+        <v>235.2</v>
       </c>
       <c r="T8" t="n">
         <v>0.045</v>
       </c>
       <c r="U8" t="n">
-        <v>0.048</v>
+        <v>0.047</v>
       </c>
       <c r="V8" t="inlineStr"/>
       <c r="W8" t="n">
@@ -1213,22 +1213,22 @@
         <v>6.82</v>
       </c>
       <c r="Z8" t="n">
-        <v>64.19</v>
+        <v>60.07</v>
       </c>
       <c r="AA8" t="n">
         <v>0</v>
       </c>
       <c r="AB8" t="n">
-        <v>0.34</v>
+        <v>0.3</v>
       </c>
       <c r="AC8" t="n">
-        <v>1.36</v>
+        <v>1.19</v>
       </c>
       <c r="AD8" t="n">
-        <v>-1.09</v>
+        <v>-1.12</v>
       </c>
       <c r="AE8" t="n">
-        <v>-1.09</v>
+        <v>-1.12</v>
       </c>
       <c r="AF8" t="n">
         <v>0.51</v>

</xml_diff>